<commit_message>
Faculty Offer letter is in progress
Faculty Offer letter is in progress
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyWork/FacultyContactDetails.xlsx
+++ b/Offline/BusinessManagement/DailyWork/FacultyContactDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\DailyWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB37BE0A-9FA7-4B96-9ADA-3F2B5ACAF68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F6D019-67B6-497D-810A-1A5C12F483D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>SlNo</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t xml:space="preserve">Dr Partha Sarathi Chakraborty </t>
+  </si>
+  <si>
+    <t>Sini Mam</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
   </si>
 </sst>
 </file>
@@ -439,7 +445,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,7 +579,24 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45126</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>8240897581</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Faculty Detail is updated
Faculty Detail is updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyWork/FacultyContactDetails.xlsx
+++ b/Offline/BusinessManagement/DailyWork/FacultyContactDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\DailyWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F6D019-67B6-497D-810A-1A5C12F483D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B667C81C-D36C-425E-B096-096267C0199B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>SlNo</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Chemistry</t>
+  </si>
+  <si>
+    <t>As she is working with Fitjee, hence it is not possible to work with other organisation</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B7" sqref="B7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,7 +460,7 @@
     <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="63.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="70.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -582,20 +585,26 @@
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="5">
         <v>45126</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>8240897581</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="6" t="s">
         <v>8</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Loreto Email Id added
Loreto Email Id added
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyWork/FacultyContactDetails.xlsx
+++ b/Offline/BusinessManagement/DailyWork/FacultyContactDetails.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\DailyWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE15C186-4D79-4DCC-9679-8C8B8268C9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3853386D-8FFC-4DFA-B9E5-432102AE4388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Faculty Contact Details" sheetId="1" r:id="rId1"/>
     <sheet name="Faculty Required" sheetId="2" r:id="rId2"/>
+    <sheet name="Loreto-Email-Id" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>SlNo</t>
   </si>
@@ -173,13 +174,16 @@
   </si>
   <si>
     <t>a) Biology / Life Science (2 teachers) --&gt; VIII to XII</t>
+  </si>
+  <si>
+    <t>leroffice@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +204,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -228,10 +240,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -247,12 +260,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -732,7 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EAD798-0DF0-4EE2-934F-0A48BED80FA1}">
   <dimension ref="C2:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -743,12 +758,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C3" s="8"/>
@@ -757,7 +772,7 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -833,4 +848,27 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E91BA0-385B-4F2E-9F21-1D4601101643}">
+  <dimension ref="D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D2" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{23082FFD-A7B8-4987-BED2-E0B7BDB04391}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
IT Product Features Added
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyWork/FacultyContactDetails.xlsx
+++ b/Offline/BusinessManagement/DailyWork/FacultyContactDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\DailyWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3853386D-8FFC-4DFA-B9E5-432102AE4388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF679A92-4425-40F2-858E-81B7169D3C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Faculty Contact Details" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>SlNo</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>leroffice@gmail.com</t>
+  </si>
+  <si>
+    <t>IT</t>
   </si>
 </sst>
 </file>
@@ -261,10 +264,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -747,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EAD798-0DF0-4EE2-934F-0A48BED80FA1}">
   <dimension ref="C2:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,12 +761,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C3" s="8"/>
@@ -777,6 +780,9 @@
       </c>
       <c r="D4" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.3">
@@ -854,14 +860,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E91BA0-385B-4F2E-9F21-1D4601101643}">
   <dimension ref="D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>